<commit_message>
Mixed type messages (uint32/floats) up and running. Mixed type store function working.
</commit_message>
<xml_diff>
--- a/apps/imputation/Imputation Placement.xlsx
+++ b/apps/imputation/Imputation Placement.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drjor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drjor\Documents\tinsel\apps\imputation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC1DB82-F389-43E2-A60B-C655EBA15715}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9139A887-F652-4F7E-9060-5E2B3446CA14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{0C236103-F992-4580-ADEB-69FDAD861B74}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>Core 0</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>3,0</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8E2218-A1A9-45C6-83A7-1D4D88E1E785}">
-  <dimension ref="A1:S117"/>
+  <dimension ref="A1:S119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="P104" sqref="P104"/>
+      <selection activeCell="N119" sqref="N119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2760,6 +2763,35 @@
         <v>31</v>
       </c>
     </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>19</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="F119">
+        <v>2</v>
+      </c>
+      <c r="G119">
+        <v>3</v>
+      </c>
+      <c r="I119">
+        <v>4</v>
+      </c>
+      <c r="J119">
+        <v>5</v>
+      </c>
+      <c r="L119">
+        <v>6</v>
+      </c>
+      <c r="M119">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>